<commit_message>
Remove old asta model
</commit_message>
<xml_diff>
--- a/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
+++ b/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edumi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CAAFF2B-55E4-43A8-858D-7268A8D69004}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E4414E-E034-4759-9F54-324FC302E8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Ver-Construção1" sheetId="5" r:id="rId5"/>
     <sheet name="Ver-Transição1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="129">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -705,15 +705,6 @@
   </si>
   <si>
     <t>Eduardo Minghini Sales da Silva</t>
-  </si>
-  <si>
-    <t>Bruno Tavares da Cunha</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t>Parcialmente</t>
   </si>
 </sst>
 </file>
@@ -1224,7 +1215,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="5B9BD5"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1277,7 +1268,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6333333333333333</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1498,7 +1489,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="5B9BD5"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1618,7 +1609,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ED7D31"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1738,7 +1729,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="A5A5A5"/>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1858,7 +1849,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC000"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -2234,34 +2225,34 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2359,7 +2350,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2451,13 +2442,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2466,13 +2457,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,7 +2543,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2567,7 +2558,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -4328,9 +4319,9 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="3" t="e">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.6333333333333333</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7416,21 +7407,21 @@
       <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>1</v>
-      </c>
-      <c r="P2" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P2" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q2" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R2" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7456,21 +7447,21 @@
       <c r="N3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>1</v>
-      </c>
-      <c r="P3" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P3" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q3" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R3" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7496,21 +7487,21 @@
       <c r="N4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>0.75</v>
-      </c>
-      <c r="P4" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q4" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>0.25</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7536,21 +7527,21 @@
       <c r="N5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P5" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q5" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R5" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7576,21 +7567,21 @@
       <c r="N6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>1</v>
-      </c>
-      <c r="P6" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q6" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R6" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -7616,21 +7607,21 @@
       <c r="N7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>0.8</v>
-      </c>
-      <c r="P7" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q7" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>0.2</v>
-      </c>
-      <c r="R7" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7656,21 +7647,21 @@
       <c r="N8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>1</v>
-      </c>
-      <c r="P8" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q8" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>0</v>
-      </c>
-      <c r="R8" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -7696,21 +7687,21 @@
       <c r="N9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="P9" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P9" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q9" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>0.33333333333333331</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7736,21 +7727,21 @@
       <c r="N10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="P10" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P10" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q10" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="R10" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R10" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7776,21 +7767,21 @@
       <c r="N11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="P11" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P11" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q11" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="R11" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7816,21 +7807,21 @@
       <c r="N12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="6" t="e">
         <f>('Ver-Elaboração1'!$G$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" s="6" t="e">
         <f>('Ver-Elaboração1'!$H$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" s="6" t="e">
         <f>('Ver-Elaboração1'!$I$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>1</v>
-      </c>
-      <c r="R12" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" s="6" t="e">
         <f>('Ver-Elaboração1'!$J$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1"/>
@@ -9345,7 +9336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:A52"/>
     </sheetView>
   </sheetViews>
@@ -14158,9 +14149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -14189,16 +14178,14 @@
         <v>30</v>
       </c>
       <c r="B2" s="30"/>
-      <c r="C2" s="8">
-        <v>45588</v>
-      </c>
+      <c r="C2" s="26"/>
       <c r="D2" s="40" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="9">
+      <c r="F2" s="9" t="e">
         <f>COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>0.6333333333333333</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1">
@@ -14206,9 +14193,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="30"/>
-      <c r="C3" s="10" t="s">
-        <v>129</v>
-      </c>
+      <c r="C3" s="10"/>
       <c r="D3" s="42" t="s">
         <v>33</v>
       </c>
@@ -14255,14 +14240,12 @@
       <c r="C6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D6" s="19"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="5">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="5">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -14295,14 +14278,12 @@
       <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D8" s="19"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="5">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="5">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -14351,14 +14332,12 @@
       <c r="C10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="5">
         <f>COUNTIF(D10:D13,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="5">
         <f>COUNTIF(D10:D13,"Parcialmente")</f>
@@ -14370,7 +14349,7 @@
       </c>
       <c r="J10" s="5">
         <f>COUNTIF(D10:D13,"NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1">
@@ -14381,9 +14360,7 @@
       <c r="C11" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D11" s="19"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -14395,9 +14372,7 @@
       <c r="C12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="D12" s="19"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
@@ -14409,9 +14384,7 @@
       <c r="C13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D13" s="19"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
     </row>
@@ -14433,9 +14406,7 @@
       <c r="C15" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D15" s="19"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="5">
@@ -14448,7 +14419,7 @@
       </c>
       <c r="I15" s="5">
         <f>COUNTIF(D15,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5">
         <f>COUNTIF(D15,"NA")</f>
@@ -14473,14 +14444,12 @@
       <c r="C17" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D17" s="19"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="5">
         <f>COUNTIF(D17,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="5">
         <f>COUNTIF(D17,"Parcialmente")</f>
@@ -14515,14 +14484,12 @@
       <c r="C19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D19" s="19"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="5">
         <f>COUNTIF(D19:D23,"Sim")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5">
         <f>COUNTIF(D19:D23,"Parcialmente")</f>
@@ -14530,7 +14497,7 @@
       </c>
       <c r="I19" s="5">
         <f>COUNTIF(D19:D23,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="5">
         <f>COUNTIF(D19:D23,"NA")</f>
@@ -14545,9 +14512,7 @@
       <c r="C20" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D20" s="19"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
     </row>
@@ -14559,9 +14524,7 @@
       <c r="C21" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D21" s="19"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="22"/>
@@ -14593,9 +14556,7 @@
       <c r="C22" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D22" s="19"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
@@ -14607,9 +14568,7 @@
       <c r="C23" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D23" s="19"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
@@ -14651,14 +14610,12 @@
       <c r="C25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D25" s="19"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="5">
         <f>COUNTIF(D25:D26,"Sim")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="5">
         <f>COUNTIF(D25:D26,"Parcialmente")</f>
@@ -14697,9 +14654,7 @@
       <c r="C26" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D26" s="19"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="22"/>
@@ -14743,18 +14698,16 @@
       <c r="C28" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D28" s="19"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="5">
         <f>COUNTIF(D28:D33,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28" s="5">
         <f>COUNTIF(D28:D33,"Parcialmente")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I28" s="5">
         <f>COUNTIF(D28:D33,"Não")</f>
@@ -14762,7 +14715,7 @@
       </c>
       <c r="J28" s="5">
         <f>COUNTIF(D28:D33,"NA")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="18.75" customHeight="1">
@@ -14773,9 +14726,7 @@
       <c r="C29" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="D29" s="19"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
     </row>
@@ -14787,9 +14738,7 @@
       <c r="C30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="D30" s="19"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
@@ -14801,9 +14750,7 @@
       <c r="C31" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="D31" s="19"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
     </row>
@@ -14815,9 +14762,7 @@
       <c r="C32" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="D32" s="19"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
     </row>
@@ -14829,9 +14774,7 @@
       <c r="C33" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>52</v>
-      </c>
+      <c r="D33" s="19"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
     </row>
@@ -14855,14 +14798,12 @@
       <c r="C35" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D35" s="19"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="5">
         <f>COUNTIF(D35:D40,"Sim")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H35" s="5">
         <f>COUNTIF(D35:D40,"Parcialmente")</f>
@@ -14870,7 +14811,7 @@
       </c>
       <c r="I35" s="5">
         <f>COUNTIF(D35:D40,"Não")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35" s="5">
         <f>COUNTIF(D35:D40,"NA")</f>
@@ -14885,9 +14826,7 @@
       <c r="C36" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D36" s="19"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
     </row>
@@ -14899,9 +14838,7 @@
       <c r="C37" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D37" s="19"/>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
     </row>
@@ -14913,9 +14850,7 @@
       <c r="C38" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D38" s="19"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
     </row>
@@ -14927,9 +14862,7 @@
       <c r="C39" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D39" s="19"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
     </row>
@@ -14941,9 +14874,7 @@
       <c r="C40" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D40" s="19"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
     </row>
@@ -14967,14 +14898,12 @@
       <c r="C42" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D42" s="19"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="5">
         <f>COUNTIF(D42:D44,"Sim")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H42" s="5">
         <f>COUNTIF(D42:D44,"Parcialmente")</f>
@@ -14982,7 +14911,7 @@
       </c>
       <c r="I42" s="5">
         <f>COUNTIF(D42:D44,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="5">
         <f>COUNTIF(D42:D44,"NA")</f>
@@ -14997,9 +14926,7 @@
       <c r="C43" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="D43" s="19"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
     </row>
@@ -15011,9 +14938,7 @@
       <c r="C44" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D44" s="19"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
@@ -15035,9 +14960,7 @@
       <c r="C46" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D46" s="19"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="5">
@@ -15050,7 +14973,7 @@
       </c>
       <c r="I46" s="5">
         <f>COUNTIF(D46:D48,"Não")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46" s="5">
         <f>COUNTIF(D46:D48,"NA")</f>
@@ -15065,9 +14988,7 @@
       <c r="C47" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D47" s="19"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
     </row>
@@ -15079,9 +15000,7 @@
       <c r="C48" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>130</v>
-      </c>
+      <c r="D48" s="19"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
     </row>
@@ -28270,11 +28189,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -28282,6 +28196,11 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D17 D19 D25 D29 D32 D35 D43 D47" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Documentação referente a fase de construção
</commit_message>
<xml_diff>
--- a/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
+++ b/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edumi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\OneDrive\Área de Trabalho\Projetos IF\Wikipedia Biologica\WBio\Wikipedia-Biologica-02\Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E4414E-E034-4759-9F54-324FC302E8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833C5582-41CE-4664-B43F-1330949D48A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,17 @@
     <sheet name="Ver-Transição1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -318,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="131">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -705,6 +716,12 @@
   </si>
   <si>
     <t>Eduardo Minghini Sales da Silva</t>
+  </si>
+  <si>
+    <t>Parcialmente</t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1232,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="5B9BD5"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1268,10 +1285,10 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>89.65517241379311</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>82.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1489,7 +1506,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="5B9BD5"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1552,7 +1569,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -1576,7 +1593,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,7 +1626,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="ED7D31"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1729,7 +1746,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="A5A5A5"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1849,7 +1866,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln cmpd="sng">
               <a:solidFill>
@@ -1912,7 +1929,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1936,7 +1953,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,34 +2245,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2454,10 +2471,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2537,7 +2554,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2552,13 +2569,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2806,37 +2823,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.7142857142857143</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2919,7 +2936,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2934,16 +2951,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -3023,7 +3040,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3044,7 +3061,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3139,25 +3156,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -4282,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4319,18 +4336,18 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="e">
-        <f>'Ver-Elaboração1'!$F$2</f>
-        <v>#DIV/0!</v>
+      <c r="B4" s="3">
+        <f>('Ver-Elaboração1'!$F$2) *100</f>
+        <v>89.65517241379311</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="e">
-        <f>'Ver-Construção1'!$F$2</f>
-        <v>#DIV/0!</v>
+      <c r="B5" s="3">
+        <f>('Ver-Construção1'!$F$2) *100</f>
+        <v>82.142857142857139</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7335,7 +7352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7407,21 +7424,21 @@
       <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="6" t="e">
+      <c r="O2" s="6">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P2" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q2" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7447,21 +7464,21 @@
       <c r="N3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="6" t="e">
+      <c r="O3" s="6">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7470,7 +7487,7 @@
       </c>
       <c r="B4" s="6">
         <f>('Ver-Iniciação1'!$G$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C4" s="6">
         <f>('Ver-Iniciação1'!$H$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
@@ -7482,26 +7499,26 @@
       </c>
       <c r="E4" s="6">
         <f>('Ver-Iniciação1'!$J$13/SUM('Ver-Iniciação1'!$G$13:'Ver-Iniciação1'!$J$13))</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="6" t="e">
+      <c r="O4" s="6">
         <f>('Ver-Elaboração1'!$G$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
         <f>('Ver-Elaboração1'!$H$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
         <f>('Ver-Elaboração1'!$I$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
         <f>('Ver-Elaboração1'!$J$10/SUM('Ver-Elaboração1'!$G$10:'Ver-Elaboração1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7527,21 +7544,21 @@
       <c r="N5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="6" t="e">
+      <c r="O5" s="6">
         <f>('Ver-Elaboração1'!$G$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
         <f>('Ver-Elaboração1'!$H$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
         <f>('Ver-Elaboração1'!$I$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
         <f>('Ver-Elaboração1'!$J$15/SUM('Ver-Elaboração1'!$G$15:'Ver-Elaboração1'!$J$15))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7567,21 +7584,21 @@
       <c r="N6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="6" t="e">
+      <c r="O6" s="6">
         <f>('Ver-Elaboração1'!$G$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P6" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
         <f>('Ver-Elaboração1'!$H$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q6" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="6">
         <f>('Ver-Elaboração1'!$I$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R6" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
         <f>('Ver-Elaboração1'!$J$17/SUM('Ver-Elaboração1'!$G$17:'Ver-Elaboração1'!$J$17))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -7607,21 +7624,21 @@
       <c r="N7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O7" s="6" t="e">
+      <c r="O7" s="6">
         <f>('Ver-Elaboração1'!$G$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="6" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="P7" s="6">
         <f>('Ver-Elaboração1'!$H$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="6">
         <f>('Ver-Elaboração1'!$I$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R7" s="6">
         <f>('Ver-Elaboração1'!$J$19/SUM('Ver-Elaboração1'!$G$19:'Ver-Elaboração1'!$J$19))</f>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7647,21 +7664,21 @@
       <c r="N8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="6" t="e">
+      <c r="O8" s="6">
         <f>('Ver-Elaboração1'!$G$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P8" s="6" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="6">
         <f>('Ver-Elaboração1'!$H$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="6">
         <f>('Ver-Elaboração1'!$I$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R8" s="6">
         <f>('Ver-Elaboração1'!$J$25/SUM('Ver-Elaboração1'!$G$25:'Ver-Elaboração1'!$J$25))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -7687,21 +7704,21 @@
       <c r="N9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="6" t="e">
+      <c r="O9" s="6">
         <f>('Ver-Elaboração1'!$G$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="6" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P9" s="6">
         <f>('Ver-Elaboração1'!$H$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
         <f>('Ver-Elaboração1'!$I$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="6" t="e">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="R9" s="6">
         <f>('Ver-Elaboração1'!$J$28/SUM('Ver-Elaboração1'!$G$28:'Ver-Elaboração1'!$J$28))</f>
-        <v>#DIV/0!</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7727,21 +7744,21 @@
       <c r="N10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="6" t="e">
+      <c r="O10" s="6">
         <f>('Ver-Elaboração1'!$G$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="6" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P10" s="6">
         <f>('Ver-Elaboração1'!$H$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6">
         <f>('Ver-Elaboração1'!$I$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="6" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="R10" s="6">
         <f>('Ver-Elaboração1'!$J$35/SUM('Ver-Elaboração1'!$G$35:'Ver-Elaboração1'!$J$35))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7767,21 +7784,21 @@
       <c r="N11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O11" s="6" t="e">
+      <c r="O11" s="6">
         <f>('Ver-Elaboração1'!$G$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6">
         <f>('Ver-Elaboração1'!$H$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="6">
         <f>('Ver-Elaboração1'!$I$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R11" s="6">
         <f>('Ver-Elaboração1'!$J$42/SUM('Ver-Elaboração1'!$G$42:'Ver-Elaboração1'!$J$42))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7790,7 +7807,7 @@
       </c>
       <c r="B12" s="6">
         <f>('Ver-Iniciação1'!$G$49/SUM('Ver-Iniciação1'!$G$49:'Ver-Iniciação1'!$J$49))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="6">
         <f>('Ver-Iniciação1'!$H$49/SUM('Ver-Iniciação1'!$G$49:'Ver-Iniciação1'!$J$49))</f>
@@ -7802,26 +7819,26 @@
       </c>
       <c r="E12" s="6">
         <f>('Ver-Iniciação1'!$J$49/SUM('Ver-Iniciação1'!$G$49:'Ver-Iniciação1'!$J$49))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="6" t="e">
+      <c r="O12" s="6">
         <f>('Ver-Elaboração1'!$G$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="6" t="e">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
         <f>('Ver-Elaboração1'!$H$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6">
         <f>('Ver-Elaboração1'!$I$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="6" t="e">
+        <v>0</v>
+      </c>
+      <c r="R12" s="6">
         <f>('Ver-Elaboração1'!$J$46/SUM('Ver-Elaboração1'!$G$46:'Ver-Elaboração1'!$J$46))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1"/>
@@ -7846,42 +7863,42 @@
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="6" t="e">
+      <c r="B23" s="6">
         <f>('Ver-Construção1'!$G$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="C23" s="7">
         <f>('Ver-Construção1'!$H$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7">
         <f>('Ver-Construção1'!$I$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7">
         <f>('Ver-Construção1'!$J$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="6" t="e">
+      <c r="B24" s="6">
         <f>('Ver-Construção1'!$G$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
         <f>('Ver-Construção1'!$H$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D24" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7">
         <f>('Ver-Construção1'!$I$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
         <f>('Ver-Construção1'!$J$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M24" s="5" t="s">
         <v>7</v>
@@ -7903,21 +7920,21 @@
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="6" t="e">
+      <c r="B25" s="6">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C25" s="7">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25" s="7">
         <f>('Ver-Construção1'!$I$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
         <f>('Ver-Construção1'!$J$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>13</v>
@@ -7943,21 +7960,21 @@
       <c r="A26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="7" t="e">
+      <c r="B26" s="7">
         <f>('Ver-Construção1'!$G$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C26" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
         <f>('Ver-Construção1'!$H$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D26" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
         <f>('Ver-Construção1'!$I$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
         <f>('Ver-Construção1'!$J$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>14</v>
@@ -7983,21 +8000,21 @@
       <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="7" t="e">
+      <c r="B27" s="7">
         <f>('Ver-Construção1'!$G$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C27" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7">
         <f>('Ver-Construção1'!$H$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D27" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
         <f>('Ver-Construção1'!$I$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
         <f>('Ver-Construção1'!$J$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>15</v>
@@ -8023,21 +8040,21 @@
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="7" t="e">
+      <c r="B28" s="7">
         <f>('Ver-Construção1'!$G$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="7" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="7">
         <f>('Ver-Construção1'!$H$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
         <f>('Ver-Construção1'!$I$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
         <f>('Ver-Construção1'!$J$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>16</v>
@@ -8063,21 +8080,21 @@
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="7" t="e">
+      <c r="B29" s="7">
         <f>('Ver-Construção1'!$G$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C29" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="C29" s="7">
         <f>('Ver-Construção1'!$H$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D29" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
         <f>('Ver-Construção1'!$I$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E29" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
         <f>('Ver-Construção1'!$J$21/SUM('Ver-Construção1'!$G$21:'Ver-Construção1'!$J$21))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M29" s="5" t="s">
         <v>17</v>
@@ -8103,21 +8120,21 @@
       <c r="A30" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="7" t="e">
+      <c r="B30" s="7">
         <f>('Ver-Construção1'!$G$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C30" s="7" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="7">
         <f>('Ver-Construção1'!$H$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D30" s="7" t="e">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D30" s="7">
         <f>('Ver-Construção1'!$I$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E30" s="7">
         <f>('Ver-Construção1'!$J$23/SUM('Ver-Construção1'!$G$23:'Ver-Construção1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M30" s="5" t="s">
         <v>18</v>
@@ -8143,21 +8160,21 @@
       <c r="A31" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="7" t="e">
+      <c r="B31" s="7">
         <f>('Ver-Construção1'!$G$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31" s="7" t="e">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C31" s="7">
         <f>('Ver-Construção1'!$H$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="7" t="e">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="D31" s="7">
         <f>('Ver-Construção1'!$I$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
         <f>('Ver-Construção1'!$J$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>22</v>
@@ -8183,21 +8200,21 @@
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="7" t="e">
+      <c r="B32" s="7">
         <f>('Ver-Construção1'!$G$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7">
         <f>('Ver-Construção1'!$H$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7">
         <f>('Ver-Construção1'!$I$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7">
         <f>('Ver-Construção1'!$J$38/SUM('Ver-Construção1'!$G$38:'Ver-Construção1'!$J$38))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M32" s="5" t="s">
         <v>26</v>
@@ -8223,21 +8240,21 @@
       <c r="A33" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="7" t="e">
+      <c r="B33" s="7">
         <f>('Ver-Construção1'!$G$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="7" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C33" s="7">
         <f>('Ver-Construção1'!$H$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D33" s="7">
         <f>('Ver-Construção1'!$I$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7">
         <f>('Ver-Construção1'!$J$45/SUM('Ver-Construção1'!$G$45:'Ver-Construção1'!$J$45))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M33" s="5" t="s">
         <v>27</v>
@@ -8263,21 +8280,21 @@
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="7" t="e">
+      <c r="B34" s="7">
         <f>('Ver-Construção1'!$G$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7">
         <f>('Ver-Construção1'!$H$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7">
         <f>('Ver-Construção1'!$I$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7">
         <f>('Ver-Construção1'!$J$49/SUM('Ver-Construção1'!$G$49:'Ver-Construção1'!$J$49))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>28</v>
@@ -9337,7 +9354,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:A52"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9587,7 +9604,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="5">
         <f>COUNTIF(D14:D18,"Sim")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="5">
         <f>COUNTIF(D14:D18,"Parcialmente")</f>
@@ -9599,7 +9616,7 @@
       </c>
       <c r="J13" s="5">
         <f>COUNTIF(D14:D18,"NA")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1">
@@ -9727,7 +9744,7 @@
         <v>53</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -10270,7 +10287,7 @@
       <c r="F49" s="16"/>
       <c r="G49" s="5">
         <f>COUNTIF(D50:D52,"Sim")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H49" s="5">
         <f>COUNTIF(D50:D52,"Parcialmente")</f>
@@ -10282,7 +10299,7 @@
       </c>
       <c r="J49" s="5">
         <f>COUNTIF(D50:D52,"NA")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="18.75" customHeight="1">
@@ -10294,7 +10311,7 @@
         <v>44</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
@@ -10308,7 +10325,7 @@
         <v>74</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
@@ -10322,7 +10339,7 @@
         <v>75</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
@@ -14149,7 +14166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -14183,9 +14202,9 @@
         <v>31</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="9" t="e">
+      <c r="F2" s="9">
         <f>COUNTIF(D5:D48,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.89655172413793105</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1">
@@ -14240,7 +14259,9 @@
       <c r="C6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="5">
@@ -14257,7 +14278,7 @@
       </c>
       <c r="J6" s="5">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="18.75" customHeight="1">
@@ -14278,12 +14299,14 @@
       <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="5">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -14314,7 +14337,7 @@
       <c r="Y8" s="22"/>
       <c r="Z8" s="22"/>
     </row>
-    <row r="9" spans="1:26" ht="18.75" customHeight="1">
+    <row r="9" spans="1:26">
       <c r="A9" s="32"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15" t="s">
@@ -14332,12 +14355,14 @@
       <c r="C10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="5">
         <f>COUNTIF(D10:D13,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10" s="5">
         <f>COUNTIF(D10:D13,"Parcialmente")</f>
@@ -14360,7 +14385,9 @@
       <c r="C11" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -14372,7 +14399,9 @@
       <c r="C12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
@@ -14384,7 +14413,9 @@
       <c r="C13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
     </row>
@@ -14406,12 +14437,14 @@
       <c r="C15" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="5">
         <f>COUNTIF(D15,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="5">
         <f>COUNTIF(D15,"Parcialmente")</f>
@@ -14444,12 +14477,14 @@
       <c r="C17" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="5">
         <f>COUNTIF(D17,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
         <f>COUNTIF(D17,"Parcialmente")</f>
@@ -14484,12 +14519,14 @@
       <c r="C19" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="5">
         <f>COUNTIF(D19:D23,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" s="5">
         <f>COUNTIF(D19:D23,"Parcialmente")</f>
@@ -14501,7 +14538,7 @@
       </c>
       <c r="J19" s="5">
         <f>COUNTIF(D19:D23,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="18.75" customHeight="1">
@@ -14512,7 +14549,9 @@
       <c r="C20" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
     </row>
@@ -14524,7 +14563,9 @@
       <c r="C21" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="22"/>
@@ -14556,7 +14597,9 @@
       <c r="C22" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
@@ -14568,7 +14611,9 @@
       <c r="C23" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
@@ -14610,12 +14655,14 @@
       <c r="C25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="5">
         <f>COUNTIF(D25:D26,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5">
         <f>COUNTIF(D25:D26,"Parcialmente")</f>
@@ -14627,7 +14674,7 @@
       </c>
       <c r="J25" s="5">
         <f>COUNTIF(D25:D26,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
@@ -14654,7 +14701,9 @@
       <c r="C26" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="22"/>
@@ -14698,12 +14747,14 @@
       <c r="C28" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="5">
         <f>COUNTIF(D28:D33,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H28" s="5">
         <f>COUNTIF(D28:D33,"Parcialmente")</f>
@@ -14711,11 +14762,11 @@
       </c>
       <c r="I28" s="5">
         <f>COUNTIF(D28:D33,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="5">
         <f>COUNTIF(D28:D33,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="18.75" customHeight="1">
@@ -14726,7 +14777,9 @@
       <c r="C29" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
     </row>
@@ -14738,7 +14791,9 @@
       <c r="C30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
     </row>
@@ -14750,7 +14805,9 @@
       <c r="C31" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
     </row>
@@ -14762,7 +14819,9 @@
       <c r="C32" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
     </row>
@@ -14774,7 +14833,9 @@
       <c r="C33" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
     </row>
@@ -14798,12 +14859,14 @@
       <c r="C35" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="5">
         <f>COUNTIF(D35:D40,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H35" s="5">
         <f>COUNTIF(D35:D40,"Parcialmente")</f>
@@ -14811,7 +14874,7 @@
       </c>
       <c r="I35" s="5">
         <f>COUNTIF(D35:D40,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35" s="5">
         <f>COUNTIF(D35:D40,"NA")</f>
@@ -14826,7 +14889,9 @@
       <c r="C36" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
     </row>
@@ -14838,7 +14903,9 @@
       <c r="C37" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
     </row>
@@ -14850,7 +14917,9 @@
       <c r="C38" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
     </row>
@@ -14862,7 +14931,9 @@
       <c r="C39" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
     </row>
@@ -14874,7 +14945,9 @@
       <c r="C40" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
     </row>
@@ -14898,12 +14971,14 @@
       <c r="C42" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="5">
         <f>COUNTIF(D42:D44,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42" s="5">
         <f>COUNTIF(D42:D44,"Parcialmente")</f>
@@ -14926,7 +15001,9 @@
       <c r="C43" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
     </row>
@@ -14938,7 +15015,9 @@
       <c r="C44" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
@@ -14960,12 +15039,14 @@
       <c r="C46" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="19"/>
+      <c r="D46" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="5">
         <f>COUNTIF(D46:D48,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5">
         <f>COUNTIF(D46:D48,"Parcialmente")</f>
@@ -14988,7 +15069,9 @@
       <c r="C47" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
     </row>
@@ -15000,7 +15083,9 @@
       <c r="C48" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
     </row>
@@ -18843,7 +18928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -18877,9 +18964,9 @@
         <v>31</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="9" t="e">
+      <c r="F2" s="9">
         <f>COUNTIF(D5:D51,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.8214285714285714</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1">
@@ -18934,7 +19021,9 @@
       <c r="C6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="5">
@@ -18947,7 +19036,7 @@
       </c>
       <c r="I6" s="5">
         <f>COUNTIF(D6,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
         <f>COUNTIF(D6,"NA")</f>
@@ -18972,12 +19061,14 @@
       <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="5">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -19026,16 +19117,18 @@
       <c r="C10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="5">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="5">
         <f>COUNTIF(D10:D12,"Não")</f>
@@ -19043,7 +19136,7 @@
       </c>
       <c r="J10" s="5">
         <f>COUNTIF(D10:D12,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1">
@@ -19054,7 +19147,9 @@
       <c r="C11" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -19066,7 +19161,9 @@
       <c r="C12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
@@ -19088,12 +19185,14 @@
       <c r="C14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="5">
         <f>COUNTIF(D14,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5">
         <f>COUNTIF(D14,"Parcialmente")</f>
@@ -19126,7 +19225,9 @@
       <c r="C16" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="5">
@@ -19143,7 +19244,7 @@
       </c>
       <c r="J16" s="5">
         <f>COUNTIF(D16,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1">
@@ -19166,12 +19267,14 @@
       <c r="C18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="5">
         <f>COUNTIF(D18:D19,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5">
         <f>COUNTIF(D18:D19,"Parcialmente")</f>
@@ -19183,7 +19286,7 @@
       </c>
       <c r="J18" s="5">
         <f>COUNTIF(D18:D19,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1">
@@ -19194,7 +19297,9 @@
       <c r="C19" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
     </row>
@@ -19236,7 +19341,9 @@
       <c r="C21" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="5">
@@ -19253,7 +19360,7 @@
       </c>
       <c r="J21" s="5">
         <f>COUNTIF(D21,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
@@ -19292,20 +19399,22 @@
       <c r="C23" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="5">
         <f>COUNTIF(D23:D28,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23" s="5">
         <f>COUNTIF(D23:D28,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="5">
         <f>COUNTIF(D23:D28,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="5">
         <f>COUNTIF(D23:D28,"NA")</f>
@@ -19320,7 +19429,9 @@
       <c r="C24" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
     </row>
@@ -19332,7 +19443,9 @@
       <c r="C25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
     </row>
@@ -19344,7 +19457,9 @@
       <c r="C26" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
     </row>
@@ -19356,7 +19471,9 @@
       <c r="C27" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
@@ -19368,7 +19485,9 @@
       <c r="C28" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
     </row>
@@ -19392,16 +19511,18 @@
       <c r="C30" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="5">
         <f>COUNTIF(D30:D36,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5">
         <f>COUNTIF(D30:D36,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="5">
         <f>COUNTIF(D30:D36,"Não")</f>
@@ -19409,7 +19530,7 @@
       </c>
       <c r="J30" s="5">
         <f>COUNTIF(D30:D36,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="18.75" customHeight="1">
@@ -19420,7 +19541,9 @@
       <c r="C31" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
     </row>
@@ -19432,7 +19555,9 @@
       <c r="C32" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
     </row>
@@ -19444,7 +19569,9 @@
       <c r="C33" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
     </row>
@@ -19456,7 +19583,9 @@
       <c r="C34" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
     </row>
@@ -19468,7 +19597,9 @@
       <c r="C35" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
     </row>
@@ -19480,7 +19611,9 @@
       <c r="C36" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
     </row>
@@ -19504,12 +19637,14 @@
       <c r="C38" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="5">
         <f>COUNTIF(D38:D43,"Sim")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H38" s="5">
         <f>COUNTIF(D38:D43,"Parcialmente")</f>
@@ -19532,7 +19667,9 @@
       <c r="C39" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
     </row>
@@ -19544,7 +19681,9 @@
       <c r="C40" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
     </row>
@@ -19556,7 +19695,9 @@
       <c r="C41" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
     </row>
@@ -19568,7 +19709,9 @@
       <c r="C42" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
@@ -19580,7 +19723,9 @@
       <c r="C43" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="19"/>
+      <c r="D43" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
     </row>
@@ -19604,16 +19749,18 @@
       <c r="C45" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="5">
         <f>COUNTIF(D45:D47,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H45" s="5">
         <f>COUNTIF(D45:D47,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="5">
         <f>COUNTIF(D45:D47,"Não")</f>
@@ -19632,7 +19779,9 @@
       <c r="C46" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="19"/>
+      <c r="D46" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
     </row>
@@ -19644,7 +19793,9 @@
       <c r="C47" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="19"/>
+      <c r="D47" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
     </row>
@@ -19666,12 +19817,14 @@
       <c r="C49" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="5">
         <f>COUNTIF(D49:D51,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H49" s="5">
         <f>COUNTIF(D49:D51,"Parcialmente")</f>
@@ -19694,7 +19847,9 @@
       <c r="C50" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="19"/>
+      <c r="D50" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
     </row>
@@ -19706,7 +19861,9 @@
       <c r="C51" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D51" s="19"/>
+      <c r="D51" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
     </row>
@@ -28189,6 +28346,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -28196,11 +28358,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D17 D19 D25 D29 D32 D35 D43 D47" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Fase de transição - adição e atualização de documentos
</commit_message>
<xml_diff>
--- a/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
+++ b/Wikipedia-Biologica-02/Gerenciamento de Projeto/WBio - Checklist Verificacao de Projeto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\OneDrive\Área de Trabalho\WBio\Wikipedia-Biologica-02\Gerenciamento de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{954730C3-7D5F-4C3C-8494-E4EE9C0280E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE3BAE4-7E4D-4E50-8037-2FDC6C499876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="130">
   <si>
     <t>IAP - Indicador de Aderência ao Processo (70% a 100%)</t>
   </si>
@@ -1277,7 +1277,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.79166666666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3411,40 +3411,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3640,7 +3640,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3649,7 +3649,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3658,7 +3658,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3670,10 +3670,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.2857142857142857</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -3762,7 +3762,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3774,10 +3774,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3786,7 +3786,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.42857142857142855</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -4340,9 +4340,9 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="e">
+      <c r="B6" s="3">
         <f>'Ver-Transição1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -7925,21 +7925,21 @@
       <c r="M25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N25" s="7" t="e">
+      <c r="N25" s="7">
         <f>('Ver-Transição1'!$G$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="O25" s="7">
         <f>('Ver-Transição1'!$H$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P25" s="7">
         <f>('Ver-Transição1'!$I$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="7">
         <f>('Ver-Transição1'!$J$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
@@ -7965,21 +7965,21 @@
       <c r="M26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N26" s="7" t="e">
+      <c r="N26" s="7">
         <f>('Ver-Transição1'!$G$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O26" s="7">
         <f>('Ver-Transição1'!$H$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P26" s="7">
         <f>('Ver-Transição1'!$I$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q26" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="7">
         <f>('Ver-Transição1'!$J$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
@@ -8005,21 +8005,21 @@
       <c r="M27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N27" s="7" t="e">
+      <c r="N27" s="7">
         <f>('Ver-Transição1'!$G$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O27" s="7">
         <f>('Ver-Transição1'!$H$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P27" s="7">
         <f>('Ver-Transição1'!$I$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q27" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="7">
         <f>('Ver-Transição1'!$J$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1">
@@ -8045,21 +8045,21 @@
       <c r="M28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="N28" s="7" t="e">
+      <c r="N28" s="7">
         <f>('Ver-Transição1'!$G$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7">
         <f>('Ver-Transição1'!$H$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="7">
         <f>('Ver-Transição1'!$I$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="7">
         <f>('Ver-Transição1'!$J$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1">
@@ -8085,21 +8085,21 @@
       <c r="M29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N29" s="7" t="e">
+      <c r="N29" s="7">
         <f>('Ver-Transição1'!$G$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O29" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O29" s="7">
         <f>('Ver-Transição1'!$H$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P29" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P29" s="7">
         <f>('Ver-Transição1'!$I$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q29" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="7">
         <f>('Ver-Transição1'!$J$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1">
@@ -8125,21 +8125,21 @@
       <c r="M30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N30" s="7" t="e">
+      <c r="N30" s="7">
         <f>('Ver-Transição1'!$G$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O30" s="7">
         <f>('Ver-Transição1'!$H$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P30" s="7">
         <f>('Ver-Transição1'!$I$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="7">
         <f>('Ver-Transição1'!$J$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
@@ -8165,21 +8165,21 @@
       <c r="M31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="7" t="e">
+      <c r="N31" s="7">
         <f>('Ver-Transição1'!$G$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="7" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="O31" s="7">
         <f>('Ver-Transição1'!$H$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P31" s="7">
         <f>('Ver-Transição1'!$I$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="7" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="Q31" s="7">
         <f>('Ver-Transição1'!$J$20/SUM('Ver-Transição1'!$G$20:'Ver-Transição1'!$J$20))</f>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
@@ -8205,21 +8205,21 @@
       <c r="M32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N32" s="7" t="e">
+      <c r="N32" s="7">
         <f>('Ver-Transição1'!$G$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O32" s="7">
         <f>('Ver-Transição1'!$H$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P32" s="7">
         <f>('Ver-Transição1'!$I$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="7">
         <f>('Ver-Transição1'!$J$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1">
@@ -8245,21 +8245,21 @@
       <c r="M33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N33" s="7" t="e">
+      <c r="N33" s="7">
         <f>('Ver-Transição1'!$G$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O33" s="7">
         <f>('Ver-Transição1'!$H$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P33" s="7">
         <f>('Ver-Transição1'!$I$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q33" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="7">
         <f>('Ver-Transição1'!$J$30/SUM('Ver-Transição1'!$G$30:'Ver-Transição1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1">
@@ -8285,84 +8285,84 @@
       <c r="M34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N34" s="6" t="e">
+      <c r="N34" s="6">
         <f>('Ver-Transição1'!$G$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O34" s="7">
         <f>('Ver-Transição1'!$H$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P34" s="7">
         <f>('Ver-Transição1'!$I$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q34" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="7">
         <f>('Ver-Transição1'!$J$33/SUM('Ver-Transição1'!$G$33:'Ver-Transição1'!$J$33))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1">
       <c r="M35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N35" s="7" t="e">
+      <c r="N35" s="7">
         <f>('Ver-Transição1'!$G$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" s="7" t="e">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="O35" s="7">
         <f>('Ver-Transição1'!$H$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P35" s="7">
         <f>('Ver-Transição1'!$I$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="7" t="e">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="Q35" s="7">
         <f>('Ver-Transição1'!$J$36/SUM('Ver-Transição1'!$G$36:'Ver-Transição1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1">
       <c r="M36" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N36" s="7" t="e">
+      <c r="N36" s="7">
         <f>('Ver-Transição1'!$G$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O36" s="7" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O36" s="7">
         <f>('Ver-Transição1'!$H$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P36" s="7">
         <f>('Ver-Transição1'!$I$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="7" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q36" s="7">
         <f>('Ver-Transição1'!$J$44/SUM('Ver-Transição1'!$G$44:'Ver-Transição1'!$J$44))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1">
       <c r="M37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N37" s="7" t="e">
+      <c r="N37" s="7">
         <f>('Ver-Transição1'!$G$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O37" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="O37" s="7">
         <f>('Ver-Transição1'!$H$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="P37" s="7">
         <f>('Ver-Transição1'!$I$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="7">
         <f>('Ver-Transição1'!$J$48/SUM('Ver-Transição1'!$G$48:'Ver-Transição1'!$J$48))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1"/>
@@ -18914,7 +18914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -23660,7 +23660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -23689,14 +23691,16 @@
         <v>30</v>
       </c>
       <c r="B2" s="30"/>
-      <c r="C2" s="26"/>
+      <c r="C2" s="8">
+        <v>45629</v>
+      </c>
       <c r="D2" s="40" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="9" t="e">
+      <c r="F2" s="9">
         <f>COUNTIF(D5:D50,"Sim")/(COUNTA(D5:D49)-COUNTIF(D5:D49,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1">
@@ -23751,7 +23755,9 @@
       <c r="C6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="5">
@@ -23764,7 +23770,7 @@
       </c>
       <c r="I6" s="5">
         <f>COUNTIF(D6,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
         <f>COUNTIF(D6,"NA")</f>
@@ -23789,12 +23795,14 @@
       <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="5">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="5">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -23843,12 +23851,14 @@
       <c r="C10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="5">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -23860,7 +23870,7 @@
       </c>
       <c r="J10" s="5">
         <f>COUNTIF(D10:D12,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1">
@@ -23871,7 +23881,9 @@
       <c r="C11" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
     </row>
@@ -23883,7 +23895,9 @@
       <c r="C12" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
@@ -23905,7 +23919,9 @@
       <c r="C14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="5">
@@ -23918,7 +23934,7 @@
       </c>
       <c r="I14" s="5">
         <f>COUNTIF(D14,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="5">
         <f>COUNTIF(D14,"NA")</f>
@@ -23943,12 +23959,14 @@
       <c r="C16" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="5">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -23983,12 +24001,14 @@
       <c r="C18" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="5">
         <f>COUNTIF(D18,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="5">
         <f>COUNTIF(D18,"Parcialmente")</f>
@@ -24023,12 +24043,14 @@
       <c r="C20" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="19"/>
+      <c r="D20" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="5">
         <f>COUNTIF(D20:D24,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" s="5">
         <f>COUNTIF(D20:D24,"Parcialmente")</f>
@@ -24036,11 +24058,11 @@
       </c>
       <c r="I20" s="5">
         <f>COUNTIF(D20:D24,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="5">
         <f>COUNTIF(D20:D24,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="18.75" customHeight="1">
@@ -24051,7 +24073,9 @@
       <c r="C21" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
     </row>
@@ -24063,7 +24087,9 @@
       <c r="C22" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
     </row>
@@ -24075,7 +24101,9 @@
       <c r="C23" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
     </row>
@@ -24087,7 +24115,9 @@
       <c r="C24" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
     </row>
@@ -24111,12 +24141,14 @@
       <c r="C26" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="5">
         <f>COUNTIF(D26:D28,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="5">
         <f>COUNTIF(D26:D28,"Parcialmente")</f>
@@ -24128,7 +24160,7 @@
       </c>
       <c r="J26" s="5">
         <f>COUNTIF(D26:D28,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="18.75" customHeight="1">
@@ -24139,7 +24171,9 @@
       <c r="C27" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
@@ -24151,7 +24185,9 @@
       <c r="C28" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
     </row>
@@ -24195,12 +24231,14 @@
       <c r="C30" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="5">
         <f>COUNTIF(D30:D31,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5">
         <f>COUNTIF(D30:D31,"Parcialmente")</f>
@@ -24239,7 +24277,9 @@
       <c r="C31" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="22"/>
@@ -24281,12 +24321,14 @@
       <c r="C33" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="5">
         <f>COUNTIF(D33:D34,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H33" s="5">
         <f>COUNTIF(D33:D34,"Parcialmente")</f>
@@ -24309,7 +24351,9 @@
       <c r="C34" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
     </row>
@@ -24333,12 +24377,14 @@
       <c r="C36" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="5">
         <f>COUNTIF(D36:D42,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5">
         <f>COUNTIF(D36:D42,"Parcialmente")</f>
@@ -24346,11 +24392,11 @@
       </c>
       <c r="I36" s="5">
         <f>COUNTIF(D36:D42,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J36" s="5">
         <f>COUNTIF(D36:D42,"NA")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="18.75" customHeight="1">
@@ -24361,7 +24407,9 @@
       <c r="C37" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
     </row>
@@ -24373,7 +24421,9 @@
       <c r="C38" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
     </row>
@@ -24385,7 +24435,9 @@
       <c r="C39" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
     </row>
@@ -24397,7 +24449,9 @@
       <c r="C40" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
     </row>
@@ -24409,7 +24463,9 @@
       <c r="C41" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D41" s="19"/>
+      <c r="D41" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
     </row>
@@ -24421,7 +24477,9 @@
       <c r="C42" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="19"/>
+      <c r="D42" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
     </row>
@@ -24445,12 +24503,14 @@
       <c r="C44" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="19"/>
+      <c r="D44" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="5">
         <f>COUNTIF(D44:D46,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H44" s="5">
         <f>COUNTIF(D44:D46,"Parcialmente")</f>
@@ -24458,7 +24518,7 @@
       </c>
       <c r="I44" s="5">
         <f>COUNTIF(D44:D46,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="5">
         <f>COUNTIF(D44:D46,"NA")</f>
@@ -24473,7 +24533,9 @@
       <c r="C45" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="19"/>
+      <c r="D45" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
     </row>
@@ -24485,7 +24547,9 @@
       <c r="C46" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="19"/>
+      <c r="D46" s="19" t="s">
+        <v>129</v>
+      </c>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
     </row>
@@ -24507,12 +24571,14 @@
       <c r="C48" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="5">
         <f>COUNTIF(D48:D50,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H48" s="5">
         <f>COUNTIF(D48:D50,"Parcialmente")</f>
@@ -24535,7 +24601,9 @@
       <c r="C49" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
     </row>
@@ -24547,7 +24615,9 @@
       <c r="C50" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="19"/>
+      <c r="D50" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
     </row>
@@ -28332,6 +28402,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:F1"/>
@@ -28339,11 +28414,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D17 D19 D25 D29 D32 D35 D43 D47" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>